<commit_message>
2019 maggio - turni fino al 4 agosto 2019
</commit_message>
<xml_diff>
--- a/2019_maggio/FERIE OPERATORI  2019.xlsx
+++ b/2019_maggio/FERIE OPERATORI  2019.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giorgio\Desktop\turniOsa_excelVBA\2019_maggio\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="20115" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13095" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -219,8 +224,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,14 +276,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -288,12 +290,24 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -340,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -372,9 +386,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,6 +438,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -581,14 +631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
@@ -598,7 +648,7 @@
     <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -613,7 +663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -628,59 +678,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6"/>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -691,65 +741,65 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="5" t="s">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="5" t="s">
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="5" t="s">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="5" t="s">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="17" spans="2:7">
+      <c r="F14" s="6"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>21</v>
@@ -764,7 +814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>4</v>
@@ -780,161 +830,161 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="E24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="E25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="E26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="E27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="2" t="s">
+      <c r="E28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="E29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>33</v>
@@ -952,7 +1002,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>4</v>
@@ -970,11 +1020,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -984,11 +1034,11 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -998,11 +1048,11 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -1012,11 +1062,11 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -1026,11 +1076,11 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -1040,11 +1090,11 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -1054,11 +1104,11 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -1068,7 +1118,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="2:7">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>43</v>
       </c>
@@ -1082,7 +1132,7 @@
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>44</v>
       </c>
@@ -1096,7 +1146,7 @@
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>45</v>
       </c>
@@ -1110,7 +1160,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="2:7">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>46</v>
       </c>
@@ -1124,7 +1174,7 @@
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="2:7">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>47</v>
       </c>
@@ -1138,7 +1188,7 @@
       </c>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="2:7">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>48</v>
       </c>
@@ -1150,7 +1200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>49</v>
       </c>
@@ -1162,7 +1212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:7">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>50</v>
       </c>
@@ -1174,7 +1224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>51</v>
       </c>
@@ -1186,7 +1236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="2:7">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
         <v>52</v>
@@ -1201,7 +1251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
         <v>4</v>
@@ -1216,7 +1266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>48</v>
       </c>
@@ -1227,7 +1277,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>49</v>
       </c>
@@ -1238,7 +1288,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>50</v>
       </c>
@@ -1249,7 +1299,7 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>51</v>
       </c>
@@ -1260,7 +1310,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>56</v>
       </c>
@@ -1273,7 +1323,7 @@
       </c>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>57</v>
       </c>
@@ -1286,7 +1336,7 @@
       </c>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="2:7">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>58</v>
       </c>
@@ -1299,7 +1349,7 @@
       </c>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="2:7">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +1360,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="2:7">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1373,7 @@
       </c>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="2:7">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>61</v>
       </c>
@@ -1336,12 +1386,12 @@
       </c>
       <c r="F64" s="2"/>
     </row>
-    <row r="67" spans="2:3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>63</v>
       </c>
@@ -1349,7 +1399,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="2:3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>65</v>
       </c>
@@ -1360,24 +1410,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>